<commit_message>
Proteção acesso às paginas e excel
</commit_message>
<xml_diff>
--- a/Requisitos projecto 2 - alunos.xlsx
+++ b/Requisitos projecto 2 - alunos.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joolu\OneDrive\Ambiente de Trabalho\Faculdade\Programacão Avançada em Java\Projetos\2_Projeto\project2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76146F55-D30B-4145-ACAA-D90CA7861ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Grupos de 2" sheetId="1" r:id="rId4"/>
+    <sheet name="Grupos de 2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjvwLhjkbzvX49I2OTz5JndRHjXtA=="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
   <si>
     <t>Grupo</t>
   </si>
@@ -123,30 +132,46 @@
   <si>
     <t>R10 - Delete activity of user activities
  (Server)</t>
+  </si>
+  <si>
+    <t>Membro</t>
+  </si>
+  <si>
+    <t>João Luís</t>
+  </si>
+  <si>
+    <t>José Castro</t>
+  </si>
+  <si>
+    <t>Pedro Domingos</t>
+  </si>
+  <si>
+    <t>Todos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -156,7 +181,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -190,7 +215,13 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -204,6 +235,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -215,6 +247,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -223,80 +257,82 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -486,305 +522,401 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="D3:E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.0"/>
-    <col customWidth="1" min="2" max="2" width="39.0"/>
-    <col customWidth="1" min="3" max="4" width="12.63"/>
-    <col customWidth="1" min="5" max="5" width="23.0"/>
-    <col customWidth="1" min="6" max="6" width="12.63"/>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="C8" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="7" t="s">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="C9" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="7" t="s">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C10" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C11" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="7" t="s">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="C12" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="7" t="s">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="C13" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="7" t="s">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="C14" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="9" t="s">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>17</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="C16" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="10" t="s">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="C17" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="10" t="s">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="C18" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="12" t="s">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="12" t="s">
+      <c r="C19" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="14" t="s">
+      <c r="C20" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="14" t="s">
+      <c r="C21" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A22" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="14" t="s">
+      <c r="C22" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A23" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="14" t="s">
+      <c r="C23" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="14" t="s">
+      <c r="C24" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A25" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="14" t="s">
+      <c r="C25" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A26" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="14" t="s">
+      <c r="C26" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="14" t="s">
+      <c r="C27" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="14" t="s">
+      <c r="C28" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="14" t="s">
+      <c r="C29" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+      <c r="C30" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1750,9 +1882,8 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>